<commit_message>
feat: create results for all runs
</commit_message>
<xml_diff>
--- a/q_branch/mcp-evaluation/results/all/aggregated_results.xlsx
+++ b/q_branch/mcp-evaluation/results/all/aggregated_results.xlsx
@@ -496,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,14 +506,13 @@
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -529,40 +528,35 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>completed_count</t>
+          <t>avg_score</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>avg_score</t>
+          <t>min_score</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>min_score</t>
+          <t>max_score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>max_score</t>
+          <t>avg_duration_sec</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>avg_duration_sec</t>
+          <t>avg_turns</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>avg_turns</t>
+          <t>avg_cost</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>avg_cost</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>total_cost</t>
         </is>
@@ -571,69 +565,63 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bash</t>
+          <t>tools-bash</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>75</v>
       </c>
       <c r="C2" t="n">
-        <v>75</v>
+        <v>79.84</v>
       </c>
       <c r="D2" t="n">
-        <v>76.59999999999999</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>93.42</v>
       </c>
       <c r="G2" t="n">
-        <v>90.69</v>
-      </c>
-      <c r="H2" t="n">
-        <v>33.05</v>
+        <v>37.81</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0.38</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>23.03</v>
+        <v>28.39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>safe-shell</t>
+          <t>tools-safe-shell</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>75</v>
       </c>
       <c r="C3" t="n">
-        <v>75</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>66.81</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>100</v>
+        <v>107.41</v>
       </c>
       <c r="G3" t="n">
-        <v>93.54000000000001</v>
-      </c>
-      <c r="H3" t="n">
-        <v>38.47</v>
+        <v>41.92</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0.4</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>26.92</v>
+        <v>29.92</v>
       </c>
     </row>
     <row r="4">
@@ -646,96 +634,87 @@
         <v>75</v>
       </c>
       <c r="C4" t="n">
-        <v>75</v>
+        <v>76.95999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>76.95999999999999</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>95.05</v>
       </c>
       <c r="G4" t="n">
-        <v>95.05</v>
-      </c>
-      <c r="H4" t="n">
         <v>45.25</v>
       </c>
+      <c r="H4" s="2" t="n">
+        <v>0.46</v>
+      </c>
       <c r="I4" s="2" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="J4" s="2" t="n">
         <v>34.36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>tools-bash</t>
+          <t>bash</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>75</v>
       </c>
       <c r="C5" t="n">
-        <v>75</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>79.84</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>100</v>
+        <v>90.69</v>
       </c>
       <c r="G5" t="n">
-        <v>93.42</v>
-      </c>
-      <c r="H5" t="n">
-        <v>37.81</v>
+        <v>33.05</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.31</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>28.39</v>
+        <v>23.03</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>tools-safe-shell</t>
+          <t>safe-shell</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>75</v>
       </c>
       <c r="C6" t="n">
-        <v>75</v>
+        <v>66.81</v>
       </c>
       <c r="D6" t="n">
-        <v>78.01000000000001</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>93.54000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>107.41</v>
-      </c>
-      <c r="H6" t="n">
-        <v>41.92</v>
+        <v>38.47</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0.36</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>29.92</v>
+        <v>26.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>